<commit_message>
added 2 excel problems
</commit_message>
<xml_diff>
--- a/problems.xlsx
+++ b/problems.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC6577F-4897-4EB7-8687-F0C26E121312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8392437-B34B-4993-AD7E-087EE143742F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="103">
   <si>
     <t>School Shopping</t>
   </si>
@@ -237,6 +239,114 @@
   <si>
     <t>Car and food total</t>
   </si>
+  <si>
+    <t>Best Printer</t>
+  </si>
+  <si>
+    <t>Epsilon</t>
+  </si>
+  <si>
+    <t>Heavy Package</t>
+  </si>
+  <si>
+    <t>Zero</t>
+  </si>
+  <si>
+    <t>Initial Pay</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Sets</t>
+  </si>
+  <si>
+    <t>Pages Printed</t>
+  </si>
+  <si>
+    <t>Pages per day</t>
+  </si>
+  <si>
+    <t>Days per week</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>Total of Pages</t>
+  </si>
+  <si>
+    <t>Pages per set</t>
+  </si>
+  <si>
+    <t>Sets Price</t>
+  </si>
+  <si>
+    <t>Total of sets</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Susan</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>Cell phone bill</t>
+  </si>
+  <si>
+    <t>X-Mobile</t>
+  </si>
+  <si>
+    <t>Veritium</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Month Payments</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Taxes and fees</t>
+  </si>
+  <si>
+    <t>Cell Phone</t>
+  </si>
+  <si>
+    <t>Total (2 years)</t>
+  </si>
+  <si>
+    <t>Internet Payments</t>
+  </si>
+  <si>
+    <t>Extra GB needed</t>
+  </si>
+  <si>
+    <t>Total price (2 years)</t>
+  </si>
+  <si>
+    <t>Extra 1GB price</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>Use of GB/month</t>
+  </si>
+  <si>
+    <t>GB given</t>
+  </si>
 </sst>
 </file>
 
@@ -246,7 +356,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,8 +379,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,6 +423,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -322,7 +456,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -345,6 +479,27 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -2210,6 +2365,1463 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Printers Cost</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja4!$B$3:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Epsilon</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Heavy Package</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Zero</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja4!$B$21:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1469</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>869</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>919</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-680B-46DF-8145-A458F38AD70D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1389527760"/>
+        <c:axId val="1389528592"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1389527760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1389528592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1389528592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1389527760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Printers Cost</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja4!$B$28:$D$28</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Epsilon</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Heavy Package</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Zero</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja4!$B$46:$D$46</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>48029</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21749</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8689</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E2E8-4854-93D7-726DD2228068}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1165551824"/>
+        <c:axId val="1165550576"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1165551824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1165550576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1165550576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1165551824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Cell phone bills</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.35968044619422573"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja5!$B$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>X-Mobile</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Veritium</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ABC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja5!$B$22:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2364</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1560</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1560</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2658-4A63-A9FC-4F0983C46F7C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="200514576"/>
+        <c:axId val="200517488"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="200514576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="200517488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="200517488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="200514576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Cell phone bills</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja5!$B$31:$D$31</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>X-Mobile</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Veritium</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ABC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja5!$B$47:$D$47</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1404</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>840</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1320</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-12AF-46C5-959D-5667C917D939}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="35628976"/>
+        <c:axId val="35629392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="35628976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="35629392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="35629392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="35628976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2410,6 +4022,166 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4414,6 +6186,2018 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5111,6 +8895,160 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF8169DA-3500-4040-87F1-F07F591977D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{910B9039-8C39-46B9-913A-C904CA48D10A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>769620</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BA33985-F73F-4EAF-BE1D-D319609DCF22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>11430</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>621030</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5478B74B-05E8-47C7-88DF-0CF7C5F05B2E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6361,7 +10299,7 @@
   </sheetPr>
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
@@ -7093,4 +11031,867 @@
   <pageSetup scale="61" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2665D76A-ACBA-44C2-85FD-44F1CFD518A6}">
+  <dimension ref="A1:D46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O42" sqref="O42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="11.89453125" customWidth="1"/>
+    <col min="3" max="3" width="12.89453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="7">
+        <v>29</v>
+      </c>
+      <c r="C5" s="7">
+        <v>149</v>
+      </c>
+      <c r="D5" s="7">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="14">
+        <v>200</v>
+      </c>
+      <c r="C8" s="14">
+        <v>1000</v>
+      </c>
+      <c r="D8" s="14">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="18">
+        <v>40</v>
+      </c>
+      <c r="C9" s="18">
+        <v>90</v>
+      </c>
+      <c r="D9" s="18">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="25">
+        <v>15</v>
+      </c>
+      <c r="C12" s="25">
+        <v>15</v>
+      </c>
+      <c r="D12" s="25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="25">
+        <v>5</v>
+      </c>
+      <c r="C13" s="25">
+        <v>5</v>
+      </c>
+      <c r="D13" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="25">
+        <v>2</v>
+      </c>
+      <c r="C14" s="25">
+        <v>2</v>
+      </c>
+      <c r="D14" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="25">
+        <f>B12*B13*48*B14</f>
+        <v>7200</v>
+      </c>
+      <c r="C15" s="25">
+        <f t="shared" ref="C15:D15" si="0">C12*C13*48*C14</f>
+        <v>7200</v>
+      </c>
+      <c r="D15" s="25">
+        <f t="shared" si="0"/>
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="27">
+        <f>ROUNDUP(B15/B8,0)</f>
+        <v>36</v>
+      </c>
+      <c r="C18" s="27">
+        <f t="shared" ref="C18:D18" si="1">ROUNDUP(C15/C8,0)</f>
+        <v>8</v>
+      </c>
+      <c r="D18" s="27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="28">
+        <f>B18*B9</f>
+        <v>1440</v>
+      </c>
+      <c r="C19" s="28">
+        <f t="shared" ref="C19:D19" si="2">C18*C9</f>
+        <v>720</v>
+      </c>
+      <c r="D19" s="28">
+        <f t="shared" si="2"/>
+        <v>370</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="2">
+        <f>B19+B5</f>
+        <v>1469</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" ref="C21:D21" si="3">C19+C5</f>
+        <v>869</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="3"/>
+        <v>919</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="7">
+        <v>29</v>
+      </c>
+      <c r="C30" s="7">
+        <v>149</v>
+      </c>
+      <c r="D30" s="7">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="14">
+        <v>200</v>
+      </c>
+      <c r="C33" s="14">
+        <v>1000</v>
+      </c>
+      <c r="D33" s="14">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="18">
+        <v>40</v>
+      </c>
+      <c r="C34" s="18">
+        <v>90</v>
+      </c>
+      <c r="D34" s="18">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="25">
+        <v>500</v>
+      </c>
+      <c r="C37" s="25">
+        <v>500</v>
+      </c>
+      <c r="D37" s="25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="25">
+        <v>5</v>
+      </c>
+      <c r="C38" s="25">
+        <v>5</v>
+      </c>
+      <c r="D38" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="25">
+        <v>2</v>
+      </c>
+      <c r="C39" s="25">
+        <v>2</v>
+      </c>
+      <c r="D39" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="25">
+        <f>B37*B38*48*B39</f>
+        <v>240000</v>
+      </c>
+      <c r="C40" s="25">
+        <f t="shared" ref="C40" si="4">C37*C38*48*C39</f>
+        <v>240000</v>
+      </c>
+      <c r="D40" s="25">
+        <f t="shared" ref="D40" si="5">D37*D38*48*D39</f>
+        <v>240000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="27">
+        <f>ROUNDUP(B40/B33,0)</f>
+        <v>1200</v>
+      </c>
+      <c r="C43" s="27">
+        <f t="shared" ref="C43:D43" si="6">ROUNDUP(C40/C33,0)</f>
+        <v>240</v>
+      </c>
+      <c r="D43" s="27">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="28">
+        <f>B43*B34</f>
+        <v>48000</v>
+      </c>
+      <c r="C44" s="28">
+        <f t="shared" ref="C44" si="7">C43*C34</f>
+        <v>21600</v>
+      </c>
+      <c r="D44" s="28">
+        <f t="shared" ref="D44" si="8">D43*D34</f>
+        <v>8140</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="2">
+        <f>B44+B30</f>
+        <v>48029</v>
+      </c>
+      <c r="C46" s="2">
+        <f t="shared" ref="C46:D46" si="9">C44+C30</f>
+        <v>21749</v>
+      </c>
+      <c r="D46" s="2">
+        <f t="shared" si="9"/>
+        <v>8689</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D963B181-249A-4A0D-A88A-8EB6C16E32F3}">
+  <dimension ref="A1:D47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="16.1015625" style="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="10">
+        <v>500</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="36">
+        <v>19</v>
+      </c>
+      <c r="C11" s="36">
+        <v>35</v>
+      </c>
+      <c r="D11" s="36">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="36">
+        <v>9.5</v>
+      </c>
+      <c r="C12" s="36">
+        <v>0</v>
+      </c>
+      <c r="D12" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="36">
+        <v>30</v>
+      </c>
+      <c r="C13" s="36">
+        <v>0</v>
+      </c>
+      <c r="D13" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="37">
+        <f>SUM(B11:B13)*24</f>
+        <v>1404</v>
+      </c>
+      <c r="C14" s="37">
+        <f t="shared" ref="C14:D14" si="0">SUM(C11:C13)*24</f>
+        <v>840</v>
+      </c>
+      <c r="D14" s="37">
+        <f t="shared" si="0"/>
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="20">
+        <v>1</v>
+      </c>
+      <c r="C17" s="20">
+        <v>1</v>
+      </c>
+      <c r="D17" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="21">
+        <v>20</v>
+      </c>
+      <c r="C18" s="21">
+        <v>15</v>
+      </c>
+      <c r="D18" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="20">
+        <f>$B4-B17</f>
+        <v>2</v>
+      </c>
+      <c r="C19" s="20">
+        <f t="shared" ref="C19:D19" si="1">$B4-C17</f>
+        <v>2</v>
+      </c>
+      <c r="D19" s="20">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="21">
+        <f>B19*B18*24</f>
+        <v>960</v>
+      </c>
+      <c r="C20" s="21">
+        <f t="shared" ref="C20:D20" si="2">C19*C18*24</f>
+        <v>720</v>
+      </c>
+      <c r="D20" s="21">
+        <f t="shared" si="2"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="41">
+        <f>SUM(B20,B14)</f>
+        <v>2364</v>
+      </c>
+      <c r="C22" s="41">
+        <f t="shared" ref="C22:D22" si="3">SUM(C20,C14)</f>
+        <v>1560</v>
+      </c>
+      <c r="D22" s="41">
+        <f t="shared" si="3"/>
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="10">
+        <v>0</v>
+      </c>
+      <c r="C33" s="10">
+        <v>500</v>
+      </c>
+      <c r="D33" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="36">
+        <v>19</v>
+      </c>
+      <c r="C36" s="36">
+        <v>35</v>
+      </c>
+      <c r="D36" s="36">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="36">
+        <v>9.5</v>
+      </c>
+      <c r="C37" s="36">
+        <v>0</v>
+      </c>
+      <c r="D37" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="36">
+        <v>30</v>
+      </c>
+      <c r="C38" s="36">
+        <v>0</v>
+      </c>
+      <c r="D38" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="37">
+        <f>SUM(B36:B38)*24</f>
+        <v>1404</v>
+      </c>
+      <c r="C39" s="37">
+        <f t="shared" ref="C39" si="4">SUM(C36:C38)*24</f>
+        <v>840</v>
+      </c>
+      <c r="D39" s="37">
+        <f t="shared" ref="D39" si="5">SUM(D36:D38)*24</f>
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" s="20">
+        <v>1</v>
+      </c>
+      <c r="C42" s="20">
+        <v>1</v>
+      </c>
+      <c r="D42" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43" s="21">
+        <v>20</v>
+      </c>
+      <c r="C43" s="21">
+        <v>15</v>
+      </c>
+      <c r="D43" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="20">
+        <f>$B29-B42</f>
+        <v>0</v>
+      </c>
+      <c r="C44" s="20">
+        <f t="shared" ref="C44:D44" si="6">$B29-C42</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" s="21">
+        <f>B44*B43*24</f>
+        <v>0</v>
+      </c>
+      <c r="C45" s="21">
+        <f t="shared" ref="C45" si="7">C44*C43*24</f>
+        <v>0</v>
+      </c>
+      <c r="D45" s="21">
+        <f t="shared" ref="D45" si="8">D44*D43*24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="41">
+        <f>SUM(B45,B39)</f>
+        <v>1404</v>
+      </c>
+      <c r="C47" s="41">
+        <f t="shared" ref="C47:D47" si="9">SUM(C45,C39)</f>
+        <v>840</v>
+      </c>
+      <c r="D47" s="41">
+        <f t="shared" si="9"/>
+        <v>1320</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>